<commit_message>
Update the data - phenotype_microbiome
</commit_message>
<xml_diff>
--- a/input/comp_mrs_dog.xlsx
+++ b/input/comp_mrs_dog.xlsx
@@ -751,7 +751,7 @@
         <v>2.801788565973822</v>
       </c>
       <c r="AN2" t="n">
-        <v>1.995075048266217</v>
+        <v>1.995075048266216</v>
       </c>
     </row>
     <row r="3">
@@ -2611,7 +2611,7 @@
         <v>2.448334961485563</v>
       </c>
       <c r="AN17" t="n">
-        <v>6.77235340969462</v>
+        <v>6.772353409694619</v>
       </c>
     </row>
     <row r="18">
@@ -2859,7 +2859,7 @@
         <v>2.254064771989529</v>
       </c>
       <c r="AN19" t="n">
-        <v>6.155808351755077</v>
+        <v>6.155808351755078</v>
       </c>
     </row>
     <row r="20">
@@ -4595,7 +4595,7 @@
         <v>3.322850010526614</v>
       </c>
       <c r="AN33" t="n">
-        <v>1.308991971926992</v>
+        <v>1.308991971926991</v>
       </c>
     </row>
     <row r="34">
@@ -5587,7 +5587,7 @@
         <v>1.204401773911864</v>
       </c>
       <c r="AN41" t="n">
-        <v>6.857073980251416</v>
+        <v>6.857073980251415</v>
       </c>
     </row>
     <row r="42">
@@ -5835,7 +5835,7 @@
         <v>2.494397362795435</v>
       </c>
       <c r="AN43" t="n">
-        <v>5.357745516553171</v>
+        <v>5.357745516553172</v>
       </c>
     </row>
     <row r="44">
@@ -7819,7 +7819,7 @@
         <v>2.824992738297468</v>
       </c>
       <c r="AN59" t="n">
-        <v>3.756324770701157</v>
+        <v>3.756324770701158</v>
       </c>
     </row>
     <row r="60">
@@ -8315,7 +8315,7 @@
         <v>2.396621156425506</v>
       </c>
       <c r="AN63" t="n">
-        <v>6.001822201980266</v>
+        <v>6.001822201980267</v>
       </c>
     </row>
     <row r="64">
@@ -8563,7 +8563,7 @@
         <v>3.229072804533929</v>
       </c>
       <c r="AN65" t="n">
-        <v>3.06107854747484</v>
+        <v>3.061078547474839</v>
       </c>
     </row>
     <row r="66">
@@ -8687,7 +8687,7 @@
         <v>2.559754237381127</v>
       </c>
       <c r="AN66" t="n">
-        <v>3.992914801431267</v>
+        <v>3.992914801431266</v>
       </c>
     </row>
     <row r="67">
@@ -8811,7 +8811,7 @@
         <v>2.988979749536568</v>
       </c>
       <c r="AN67" t="n">
-        <v>2.015122586290862</v>
+        <v>2.015122586290861</v>
       </c>
     </row>
     <row r="68">
@@ -9183,7 +9183,7 @@
         <v>2.079037696280881</v>
       </c>
       <c r="AN70" t="n">
-        <v>0.5448923195780147</v>
+        <v>0.5448923195780142</v>
       </c>
     </row>
     <row r="71">
@@ -9307,7 +9307,7 @@
         <v>2.711267782049019</v>
       </c>
       <c r="AN71" t="n">
-        <v>-0.3526722819993511</v>
+        <v>-0.3526722819993515</v>
       </c>
     </row>
     <row r="72">
@@ -9927,7 +9927,7 @@
         <v>2.373054628544904</v>
       </c>
       <c r="AN76" t="n">
-        <v>0.3096618194192815</v>
+        <v>0.3096618194192819</v>
       </c>
     </row>
     <row r="77">
@@ -10051,7 +10051,7 @@
         <v>1.85321162898101</v>
       </c>
       <c r="AN77" t="n">
-        <v>-0.02763972147925653</v>
+        <v>-0.02763972147925631</v>
       </c>
     </row>
     <row r="78">
@@ -10175,7 +10175,7 @@
         <v>2.366002688000143</v>
       </c>
       <c r="AN78" t="n">
-        <v>0.9310093253572265</v>
+        <v>0.9310093253572269</v>
       </c>
     </row>
     <row r="79">
@@ -11663,7 +11663,7 @@
         <v>2.433918121628596</v>
       </c>
       <c r="AN90" t="n">
-        <v>1.067195274240549</v>
+        <v>1.06719527424055</v>
       </c>
     </row>
     <row r="91">
@@ -11911,7 +11911,7 @@
         <v>2.606532721370237</v>
       </c>
       <c r="AN92" t="n">
-        <v>0.907641720156859</v>
+        <v>0.9076417201568594</v>
       </c>
     </row>
     <row r="93">
@@ -12779,7 +12779,7 @@
         <v>2.645633434644179</v>
       </c>
       <c r="AN99" t="n">
-        <v>2.451030312406533</v>
+        <v>2.451030312406532</v>
       </c>
     </row>
     <row r="100">
@@ -12903,7 +12903,7 @@
         <v>2.553406261296868</v>
       </c>
       <c r="AN100" t="n">
-        <v>3.344240840964734</v>
+        <v>3.344240840964733</v>
       </c>
     </row>
     <row r="101">

</xml_diff>